<commit_message>
Updated tissue weights script for HPD
</commit_message>
<xml_diff>
--- a/Mouse Data/HPD/HPD fat pad weights.xlsx
+++ b/Mouse Data/HPD/HPD fat pad weights.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fat pad wts" sheetId="1" r:id="rId1"/>
     <sheet name="water" sheetId="2" r:id="rId2"/>
     <sheet name="Muscle wts" sheetId="3" r:id="rId3"/>
+    <sheet name="Tissue Weight Summary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>CD</t>
   </si>
@@ -132,6 +133,45 @@
   </si>
   <si>
     <t>Ttest</t>
+  </si>
+  <si>
+    <t>Right.EWAT</t>
+  </si>
+  <si>
+    <t>Left EWAT</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Control Diet</t>
+  </si>
+  <si>
+    <t>High Protein Diet</t>
+  </si>
+  <si>
+    <t>Right.IWAT</t>
+  </si>
+  <si>
+    <t>Left.IWAT</t>
+  </si>
+  <si>
+    <t>Body Weight</t>
+  </si>
+  <si>
+    <t>Right.Quad</t>
+  </si>
+  <si>
+    <t>Left.Quad</t>
+  </si>
+  <si>
+    <t>TS.Left</t>
+  </si>
+  <si>
+    <t>TS.Right</t>
   </si>
 </sst>
 </file>
@@ -187,8 +227,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -206,19 +258,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,11 +490,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118943320"/>
-        <c:axId val="2118946296"/>
+        <c:axId val="2138578728"/>
+        <c:axId val="2138581704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118943320"/>
+        <c:axId val="2138578728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -439,7 +503,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118946296"/>
+        <c:crossAx val="2138581704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -447,7 +511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118946296"/>
+        <c:axId val="2138581704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,7 +540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118943320"/>
+        <c:crossAx val="2138578728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -720,11 +784,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2114692840"/>
-        <c:axId val="2114695800"/>
+        <c:axId val="2136303320"/>
+        <c:axId val="2136306312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2114692840"/>
+        <c:axId val="2136303320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,12 +798,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114695800"/>
+        <c:crossAx val="2136306312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2114695800"/>
+        <c:axId val="2136306312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,13 +813,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114692840"/>
+        <c:crossAx val="2136303320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -994,11 +1059,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2119741896"/>
-        <c:axId val="2119744904"/>
+        <c:axId val="2106929720"/>
+        <c:axId val="2106932728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2119741896"/>
+        <c:axId val="2106929720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1082,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119744904"/>
+        <c:crossAx val="2106932728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119744904"/>
+        <c:axId val="2106932728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119741896"/>
+        <c:crossAx val="2106929720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1529,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2757,7 +2822,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="A3" sqref="A3:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3186,4 +3251,413 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>2774</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>1081.9000000000001</v>
+      </c>
+      <c r="E2">
+        <v>1075.2</v>
+      </c>
+      <c r="F2">
+        <v>607.4</v>
+      </c>
+      <c r="G2">
+        <v>676.6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>236.9</v>
+      </c>
+      <c r="I2">
+        <v>235.4</v>
+      </c>
+      <c r="J2">
+        <v>173.5</v>
+      </c>
+      <c r="K2">
+        <v>187.4</v>
+      </c>
+      <c r="L2">
+        <v>126.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>2777</v>
+      </c>
+      <c r="C3">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="D3">
+        <v>458.9</v>
+      </c>
+      <c r="E3">
+        <v>548.4</v>
+      </c>
+      <c r="F3">
+        <v>288</v>
+      </c>
+      <c r="G3">
+        <v>270.2</v>
+      </c>
+      <c r="H3">
+        <v>279.3</v>
+      </c>
+      <c r="I3">
+        <v>248.9</v>
+      </c>
+      <c r="J3">
+        <v>182.9</v>
+      </c>
+      <c r="K3">
+        <v>181.5</v>
+      </c>
+      <c r="L3">
+        <v>127.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>2778</v>
+      </c>
+      <c r="C4">
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>2792</v>
+      </c>
+      <c r="C5">
+        <v>41.2</v>
+      </c>
+      <c r="D5">
+        <v>1214.5999999999999</v>
+      </c>
+      <c r="E5">
+        <v>936.9</v>
+      </c>
+      <c r="F5">
+        <v>603.6</v>
+      </c>
+      <c r="G5">
+        <v>577.9</v>
+      </c>
+      <c r="H5">
+        <v>224</v>
+      </c>
+      <c r="I5">
+        <v>228.4</v>
+      </c>
+      <c r="J5">
+        <v>164.7</v>
+      </c>
+      <c r="K5">
+        <v>133</v>
+      </c>
+      <c r="L5">
+        <v>122.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>2791</v>
+      </c>
+      <c r="C6">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>2797</v>
+      </c>
+      <c r="C7">
+        <v>30.8</v>
+      </c>
+      <c r="D7">
+        <v>267.7</v>
+      </c>
+      <c r="E7">
+        <v>248.6</v>
+      </c>
+      <c r="F7">
+        <v>185.6</v>
+      </c>
+      <c r="G7">
+        <v>184.5</v>
+      </c>
+      <c r="H7">
+        <v>223.9</v>
+      </c>
+      <c r="I7">
+        <v>241.8</v>
+      </c>
+      <c r="J7">
+        <v>171.9</v>
+      </c>
+      <c r="K7">
+        <v>173.6</v>
+      </c>
+      <c r="L7">
+        <v>129.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>2776</v>
+      </c>
+      <c r="C8">
+        <v>30.1</v>
+      </c>
+      <c r="D8">
+        <v>197.3</v>
+      </c>
+      <c r="E8">
+        <v>213.3</v>
+      </c>
+      <c r="F8">
+        <v>103.2</v>
+      </c>
+      <c r="G8">
+        <v>118.5</v>
+      </c>
+      <c r="H8">
+        <v>258.2</v>
+      </c>
+      <c r="I8">
+        <v>255.9</v>
+      </c>
+      <c r="J8">
+        <v>188.1</v>
+      </c>
+      <c r="K8">
+        <v>173.7</v>
+      </c>
+      <c r="L8">
+        <v>142.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <v>2784</v>
+      </c>
+      <c r="C9">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>2781</v>
+      </c>
+      <c r="C10">
+        <v>31.4</v>
+      </c>
+      <c r="D10">
+        <v>575.4</v>
+      </c>
+      <c r="E10">
+        <v>548.79999999999995</v>
+      </c>
+      <c r="F10">
+        <v>348.8</v>
+      </c>
+      <c r="G10">
+        <v>327.5</v>
+      </c>
+      <c r="H10">
+        <v>265.3</v>
+      </c>
+      <c r="I10">
+        <v>249.4</v>
+      </c>
+      <c r="J10">
+        <v>200.1</v>
+      </c>
+      <c r="K10">
+        <v>195.2</v>
+      </c>
+      <c r="L10">
+        <v>133.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>2790</v>
+      </c>
+      <c r="C11">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="D11">
+        <v>597.4</v>
+      </c>
+      <c r="E11">
+        <v>664.5</v>
+      </c>
+      <c r="F11">
+        <v>401.9</v>
+      </c>
+      <c r="G11">
+        <v>391.5</v>
+      </c>
+      <c r="H11">
+        <v>273.8</v>
+      </c>
+      <c r="I11">
+        <v>249.8</v>
+      </c>
+      <c r="J11">
+        <v>202.2</v>
+      </c>
+      <c r="K11">
+        <v>196.2</v>
+      </c>
+      <c r="L11">
+        <v>141.19999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>2795</v>
+      </c>
+      <c r="C12">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D12">
+        <v>221.7</v>
+      </c>
+      <c r="E12">
+        <v>236.6</v>
+      </c>
+      <c r="F12">
+        <v>168.5</v>
+      </c>
+      <c r="G12">
+        <v>149.69999999999999</v>
+      </c>
+      <c r="H12">
+        <v>262.3</v>
+      </c>
+      <c r="I12">
+        <v>249.6</v>
+      </c>
+      <c r="J12">
+        <v>176.7</v>
+      </c>
+      <c r="K12">
+        <v>181.6</v>
+      </c>
+      <c r="L12">
+        <v>124.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>2796</v>
+      </c>
+      <c r="C13">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>